<commit_message>
feat: add name list, price list, history list
</commit_message>
<xml_diff>
--- a/namelist_template.xlsx
+++ b/namelist_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtk_yu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ETH_FAN\Documents\Code\NFPM_LuckyDraw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30F9EE64-CBC9-4AAE-9F36-0237E8816407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7D2233-B44C-4E7E-8B82-2EF140D486BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{43923C27-27DD-4BB9-9EC4-6966B899A6E7}"/>
+    <workbookView xWindow="-45120" yWindow="-6705" windowWidth="16440" windowHeight="28440" xr2:uid="{43923C27-27DD-4BB9-9EC4-6966B899A6E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
   <si>
     <t>Id</t>
   </si>
@@ -63,6 +63,102 @@
   <si>
     <t>N/A</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Natasha Haines</t>
+  </si>
+  <si>
+    <t>Leon Rodgers</t>
+  </si>
+  <si>
+    <t>Gemma Kennedy</t>
+  </si>
+  <si>
+    <t>Kiera Leblanc</t>
+  </si>
+  <si>
+    <t>Kurtis Reyes</t>
+  </si>
+  <si>
+    <t>Tommy Garcia</t>
+  </si>
+  <si>
+    <t>Camilla Woodward</t>
+  </si>
+  <si>
+    <t>Mariam Frank</t>
+  </si>
+  <si>
+    <t>Danielle Harding</t>
+  </si>
+  <si>
+    <t>Umair Tucker</t>
+  </si>
+  <si>
+    <t>Lilia Mclaughlin</t>
+  </si>
+  <si>
+    <t>Kevin Benton</t>
+  </si>
+  <si>
+    <t>Jessie Potts</t>
+  </si>
+  <si>
+    <t>Keira Dickson</t>
+  </si>
+  <si>
+    <t>Monica Arias</t>
+  </si>
+  <si>
+    <t>Phoenix Moody</t>
+  </si>
+  <si>
+    <t>Adriana Carr</t>
+  </si>
+  <si>
+    <t>Asiya Mullins</t>
+  </si>
+  <si>
+    <t>Sabrina Robertson</t>
+  </si>
+  <si>
+    <t>Layton Ellis</t>
+  </si>
+  <si>
+    <t>Lucy Zimmerman</t>
+  </si>
+  <si>
+    <t>Bridie Jensen</t>
+  </si>
+  <si>
+    <t>Ivan David</t>
+  </si>
+  <si>
+    <t>Mohammed Mccann</t>
+  </si>
+  <si>
+    <t>Dylan Camacho</t>
+  </si>
+  <si>
+    <t>Bernard Davies</t>
+  </si>
+  <si>
+    <t>Isaac Stone</t>
+  </si>
+  <si>
+    <t>Estelle Stevens</t>
+  </si>
+  <si>
+    <t>Pippa Stafford</t>
+  </si>
+  <si>
+    <t>Ifan Becker</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>AIR</t>
   </si>
 </sst>
 </file>
@@ -73,14 +169,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -115,7 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -450,10 +546,14 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -474,6 +574,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
+        <f>ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -483,221 +584,551 @@
         <v>6</v>
       </c>
       <c r="D2" s="1">
-        <v>1234</v>
+        <v>20200001</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="1">
+        <f t="shared" ref="A3:A32" si="0">ROW()-1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>20200002</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>20200003</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>20200004</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1">
+        <v>20200005</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>20200006</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20200007</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1">
+        <v>20200008</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1">
+        <v>20200009</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1">
+        <v>20200010</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1">
+        <v>20200011</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1">
+        <v>20200012</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1">
+        <v>20200013</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1">
+        <v>20200014</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1">
+        <v>20200015</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1">
+        <v>20200016</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="1">
+        <v>20200017</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1">
+        <v>20200018</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1">
+        <v>20200019</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1">
+        <v>20200020</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1">
+        <v>20200021</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1">
+        <v>20200022</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="1">
+        <v>20200023</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="1">
+        <v>20200024</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1">
+        <v>20200025</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="1">
+        <v>20200026</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="1">
+        <v>20200027</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="1">
+        <v>20200028</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="1">
+        <v>20200029</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="1">
+        <v>20200030</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="1">
+        <v>20200031</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>

</xml_diff>